<commit_message>
saved US population Death Penalty predictions
</commit_message>
<xml_diff>
--- a/data/predictions/crim_justice/death_penalty/USpop.xlsx
+++ b/data/predictions/crim_justice/death_penalty/USpop.xlsx
@@ -14,15 +14,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Favor</t>
+  </si>
+  <si>
+    <t>Predicted Favor</t>
   </si>
   <si>
     <t>Oppose</t>
   </si>
   <si>
-    <t>year</t>
+    <t>Predicted Oppose</t>
   </si>
 </sst>
 </file>
@@ -380,361 +383,430 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
+    <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>1972</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>1973</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>1974</v>
       </c>
       <c r="B4">
         <v>0.6635473653901526</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>0.3364526346098474</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:5">
       <c r="A5" s="1">
         <v>1975</v>
       </c>
       <c r="B5">
         <v>0.6433218802544045</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>0.3566781197455954</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:5">
       <c r="A6" s="1">
         <v>1976</v>
       </c>
       <c r="B6">
         <v>0.6970900376583362</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>0.3029099623416638</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:5">
       <c r="A7" s="1">
         <v>1977</v>
       </c>
       <c r="B7">
         <v>0.7212267401791868</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>0.2787732598208132</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:5">
       <c r="A8" s="1">
         <v>1978</v>
       </c>
       <c r="B8">
         <v>0.7056156260899895</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>0.2943843739100105</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:5">
       <c r="A9" s="1">
         <v>1980</v>
       </c>
       <c r="B9">
         <v>0.7202534443380241</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>0.279746555661976</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:5">
       <c r="A10" s="1">
         <v>1982</v>
       </c>
       <c r="B10">
         <v>0.7267007702710648</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>0.2732992297289352</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:5">
       <c r="A11" s="1">
         <v>1983</v>
       </c>
       <c r="B11">
         <v>0.7760797342192691</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>0.2239202657807309</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:5">
       <c r="A12" s="1">
         <v>1984</v>
       </c>
       <c r="B12">
         <v>0.7631989307195366</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>0.2368010692804633</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:5">
       <c r="A13" s="1">
         <v>1985</v>
       </c>
       <c r="B13">
         <v>0.7910992559314896</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>0.2089007440685104</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:5">
       <c r="A14" s="1">
         <v>1986</v>
       </c>
       <c r="B14">
         <v>0.7562568008705114</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>0.2437431991294886</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:5">
       <c r="A15" s="1">
         <v>1987</v>
       </c>
       <c r="B15">
         <v>0.6874590408102472</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>0.3125409591897528</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:5">
       <c r="A16" s="1">
         <v>1988</v>
       </c>
       <c r="B16">
         <v>0.7632638389647736</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>0.2367361610352265</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:4">
       <c r="A17" s="1">
         <v>1989</v>
       </c>
       <c r="B17">
         <v>0.7792928937934912</v>
       </c>
-      <c r="C17">
+      <c r="D17">
         <v>0.2207071062065087</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:4">
       <c r="A18" s="1">
         <v>1990</v>
       </c>
       <c r="B18">
         <v>0.7921878597191313</v>
       </c>
-      <c r="C18">
+      <c r="D18">
         <v>0.2078121402808687</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:4">
       <c r="A19" s="1">
         <v>1991</v>
       </c>
       <c r="B19">
         <v>0.7622108867304871</v>
       </c>
-      <c r="C19">
+      <c r="D19">
         <v>0.237789113269513</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:4">
       <c r="A20" s="1">
         <v>1993</v>
       </c>
       <c r="B20">
         <v>0.7759836551769591</v>
       </c>
-      <c r="C20">
+      <c r="D20">
         <v>0.2240163448230409</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:4">
       <c r="A21" s="1">
         <v>1994</v>
       </c>
       <c r="B21">
         <v>0.7977705294096563</v>
       </c>
-      <c r="C21">
+      <c r="D21">
         <v>0.2022294705903437</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:4">
       <c r="A22" s="1">
         <v>1996</v>
       </c>
       <c r="B22">
         <v>0.7786482737939049</v>
       </c>
-      <c r="C22">
+      <c r="D22">
         <v>0.2213517262060951</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:4">
       <c r="A23" s="1">
         <v>1998</v>
       </c>
       <c r="B23">
         <v>0.7343224456237387</v>
       </c>
-      <c r="C23">
+      <c r="D23">
         <v>0.2656775543762613</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:4">
       <c r="A24" s="1">
         <v>2000</v>
       </c>
       <c r="B24">
         <v>0.6966061562746646</v>
       </c>
-      <c r="C24">
+      <c r="D24">
         <v>0.3033938437253355</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:4">
       <c r="A25" s="1">
         <v>2002</v>
       </c>
       <c r="B25">
         <v>0.6970454545454545</v>
       </c>
-      <c r="C25">
+      <c r="D25">
         <v>0.3029545454545455</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:4">
       <c r="A26" s="1">
         <v>2004</v>
       </c>
       <c r="B26">
         <v>0.6834998002397124</v>
       </c>
-      <c r="C26">
+      <c r="D26">
         <v>0.3165001997602876</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:4">
       <c r="A27" s="1">
         <v>2006</v>
       </c>
       <c r="B27">
         <v>0.6917354493605866</v>
       </c>
-      <c r="C27">
+      <c r="D27">
         <v>0.3082645506394134</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:4">
       <c r="A28" s="1">
         <v>2008</v>
       </c>
       <c r="B28">
         <v>0.676804286164513</v>
       </c>
-      <c r="C28">
+      <c r="D28">
         <v>0.3231957138354869</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:4">
       <c r="A29" s="1">
         <v>2010</v>
       </c>
       <c r="B29">
         <v>0.6776855215360664</v>
       </c>
-      <c r="C29">
+      <c r="D29">
         <v>0.3223144784639336</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:4">
       <c r="A30" s="1">
         <v>2012</v>
       </c>
       <c r="B30">
         <v>0.6506037504868956</v>
       </c>
-      <c r="C30">
+      <c r="D30">
         <v>0.3493962495131044</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:4">
       <c r="A31" s="1">
         <v>2014</v>
       </c>
       <c r="B31">
         <v>0.6504719366256532</v>
       </c>
-      <c r="C31">
+      <c r="D31">
         <v>0.3495280633743469</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:4">
       <c r="A32" s="1">
         <v>2016</v>
       </c>
       <c r="B32">
         <v>0.6096934158612951</v>
       </c>
-      <c r="C32">
+      <c r="D32">
         <v>0.3903065841387049</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:5">
       <c r="A33" s="1">
         <v>2018</v>
       </c>
       <c r="B33">
         <v>0.6354099269803124</v>
       </c>
-      <c r="C33">
+      <c r="D33">
         <v>0.3645900730196876</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="1">
+        <v>2019</v>
+      </c>
+      <c r="C34">
+        <v>0.6336356780376812</v>
+      </c>
+      <c r="E34">
+        <v>0.3663643056059697</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="1">
+        <v>2020</v>
+      </c>
+      <c r="C35">
+        <v>0.6323061555557529</v>
+      </c>
+      <c r="E35">
+        <v>0.3676938167690059</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="1">
+        <v>2021</v>
+      </c>
+      <c r="C36">
+        <v>0.6311282812561586</v>
+      </c>
+      <c r="E36">
+        <v>0.3688716812173663</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="1">
+        <v>2022</v>
+      </c>
+      <c r="C37">
+        <v>0.6300021177793673</v>
+      </c>
+      <c r="E37">
+        <v>0.3699978352581099</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="1">
+        <v>2023</v>
+      </c>
+      <c r="C38">
+        <v>0.6288935872814473</v>
+      </c>
+      <c r="E38">
+        <v>0.3711063564324797</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="1">
+        <v>2024</v>
+      </c>
+      <c r="C39">
+        <v>0.6277910694889344</v>
+      </c>
+      <c r="E39">
+        <v>0.3722088649298879</v>
       </c>
     </row>
   </sheetData>

</xml_diff>